<commit_message>
Tablas de confusión (Issue #60)
He sacado las matrices de confusión que faltaban de las pruebas hechas inicialmente de class weight compute y data augmentation.
</commit_message>
<xml_diff>
--- a/Resultados/Class Weight Compute/Resultados Class Weight Compute.xlsx
+++ b/Resultados/Class Weight Compute/Resultados Class Weight Compute.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\TFG\Transfer-Learning-EDM\Resultados\Class Weight Compute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CE4926-FB2F-4BD9-93A8-304DA8BF8B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AA27C3-489D-4296-BBAC-963BE7A003AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holdout rgb 16batch" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="386">
   <si>
     <t>Samsung</t>
   </si>
@@ -801,9 +801,6 @@
     <t>[[5 4] [4 8]]</t>
   </si>
   <si>
-    <t>[[0 4] 16]]</t>
-  </si>
-  <si>
     <t>[[2 7] [4 8]]</t>
   </si>
   <si>
@@ -952,6 +949,252 @@
   </si>
   <si>
     <t>[[2 2] [5 10]]</t>
+  </si>
+  <si>
+    <t>[[24 14] [28 27]]</t>
+  </si>
+  <si>
+    <t>[[9 15] [9 66]]</t>
+  </si>
+  <si>
+    <t>[[18 20] [18 37]]</t>
+  </si>
+  <si>
+    <t>[[7 17] [21 54]]</t>
+  </si>
+  <si>
+    <t>[[19 19] [31 24]]</t>
+  </si>
+  <si>
+    <t>[[10 14] [16 59]]</t>
+  </si>
+  <si>
+    <t>[[23 15] [23 32]]</t>
+  </si>
+  <si>
+    <t>[[10 14] [23 52]]</t>
+  </si>
+  <si>
+    <t>[[18 20] [12 43]]</t>
+  </si>
+  <si>
+    <t>[[6 18] [6 69]]</t>
+  </si>
+  <si>
+    <t>[[17 21] [11 44]]</t>
+  </si>
+  <si>
+    <t>[[6 18] [8 67]]</t>
+  </si>
+  <si>
+    <t>[[19 19] [18 37]]</t>
+  </si>
+  <si>
+    <t>[[7 17] [13 62]]</t>
+  </si>
+  <si>
+    <t>[[7 17] [9 66]]</t>
+  </si>
+  <si>
+    <t>[[19 19] [20 35]]</t>
+  </si>
+  <si>
+    <t>[[8 16] [8 67]]</t>
+  </si>
+  <si>
+    <t>[[22 16] [32 23]]</t>
+  </si>
+  <si>
+    <t>[[11 13] [17 58]]</t>
+  </si>
+  <si>
+    <t>[[26 12] [22 33]]</t>
+  </si>
+  <si>
+    <t>[[14 10] [24 51]]</t>
+  </si>
+  <si>
+    <t>[[12 26] [20 35]]</t>
+  </si>
+  <si>
+    <t>[[8 16] [11 64]]</t>
+  </si>
+  <si>
+    <t>[[16 22] [15 40]]</t>
+  </si>
+  <si>
+    <t>[[6 18] [12 63]]</t>
+  </si>
+  <si>
+    <t>[[17 21] [27 28]]</t>
+  </si>
+  <si>
+    <t>[[4 20] [9 66]]</t>
+  </si>
+  <si>
+    <t>[[14 24] [17 38]]</t>
+  </si>
+  <si>
+    <t>[[8 16] [7 68]]</t>
+  </si>
+  <si>
+    <t>[[23 15] [22 33]]</t>
+  </si>
+  <si>
+    <t>[[8 16] [13 62]]</t>
+  </si>
+  <si>
+    <t>[[17 21] [13 42]]</t>
+  </si>
+  <si>
+    <t>[[4 20] [2 73]]</t>
+  </si>
+  <si>
+    <t>[[6 18] [9 66]]</t>
+  </si>
+  <si>
+    <t>[[17 21] [20 35]]</t>
+  </si>
+  <si>
+    <t>[[2 22] [6 69]]</t>
+  </si>
+  <si>
+    <t>[[16 22] [20 35]]</t>
+  </si>
+  <si>
+    <t>[[18 20] [16 39]]</t>
+  </si>
+  <si>
+    <t>[[10 14] [10 65]]</t>
+  </si>
+  <si>
+    <t>[[17 21] [12 43]]</t>
+  </si>
+  <si>
+    <t>[[10 14] [9 66]]</t>
+  </si>
+  <si>
+    <t>[[26 11] [27 42]]</t>
+  </si>
+  <si>
+    <t>[[17 16] [17 62]]</t>
+  </si>
+  <si>
+    <t>[[22 22] [17 45]]</t>
+  </si>
+  <si>
+    <t>[[7 21] [12 71]]</t>
+  </si>
+  <si>
+    <t>[[22 22] [22 40]]</t>
+  </si>
+  <si>
+    <t>[[8 20] [15 69]]</t>
+  </si>
+  <si>
+    <t>[[20 26] [21 41]]</t>
+  </si>
+  <si>
+    <t>[[6 22] [10 74]]</t>
+  </si>
+  <si>
+    <t>[[26 18] [19 43]]</t>
+  </si>
+  <si>
+    <t>[[8 20] [10 74]]</t>
+  </si>
+  <si>
+    <t>[[21 23] [14 48]]</t>
+  </si>
+  <si>
+    <t>[[9 19] [10 74]]</t>
+  </si>
+  <si>
+    <t>[[25 20] [31 31]]</t>
+  </si>
+  <si>
+    <t>[[9 19] [19 65]]</t>
+  </si>
+  <si>
+    <t>[[20 24] [25 37]]</t>
+  </si>
+  <si>
+    <t>[[8 20] [11 73]]</t>
+  </si>
+  <si>
+    <t>[[25 19] [24 38]]</t>
+  </si>
+  <si>
+    <t>[[10 18] [14 70]]</t>
+  </si>
+  <si>
+    <t>[[21 23] [17 45]]</t>
+  </si>
+  <si>
+    <t>[[12 16] [15 69]]</t>
+  </si>
+  <si>
+    <t>[[14 30] [19 43]]</t>
+  </si>
+  <si>
+    <t>[[9 19] [11 73]]</t>
+  </si>
+  <si>
+    <t>[[17 27] [14 48]]</t>
+  </si>
+  <si>
+    <t>[[22 22] [19 43]]</t>
+  </si>
+  <si>
+    <t>[[6 22] [2 76]]</t>
+  </si>
+  <si>
+    <t>[[0 4] [216]]</t>
+  </si>
+  <si>
+    <t>[[23 21] [24 38]]</t>
+  </si>
+  <si>
+    <t>[[11 17] [16 68]]</t>
+  </si>
+  <si>
+    <t>[[27 17] [17 45]]</t>
+  </si>
+  <si>
+    <t>[[9 19] [7 77]]</t>
+  </si>
+  <si>
+    <t>[[23 21] [19 43]]</t>
+  </si>
+  <si>
+    <t>[[17 27] [22 40]]</t>
+  </si>
+  <si>
+    <t>[[5 23] [14 70]]</t>
+  </si>
+  <si>
+    <t>[[15 29] [23 39]]</t>
+  </si>
+  <si>
+    <t>[[5 23] [7 77]]</t>
+  </si>
+  <si>
+    <t>[[26 18] [32 30]]</t>
+  </si>
+  <si>
+    <t>[[7 21] [17 67]]</t>
+  </si>
+  <si>
+    <t>[[23 21] [27 35]]</t>
+  </si>
+  <si>
+    <t>[[10 18] [13 71]]</t>
+  </si>
+  <si>
+    <t>[[21 23] [18 44]]</t>
+  </si>
+  <si>
+    <t>[[14 14] [17 67]]</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1168,7 +1411,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1178,7 +1420,20 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1190,22 +1445,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1213,6 +1452,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1504,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView topLeftCell="F69" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,16 +1776,16 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
@@ -1572,10 +1814,10 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -1594,8 +1836,8 @@
       <c r="I7" s="3">
         <v>0.83</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
@@ -1969,16 +2211,16 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="16" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D27" s="1" t="s">
@@ -2007,10 +2249,10 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="19"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -2029,8 +2271,8 @@
       <c r="I28" s="3">
         <v>0.83</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
@@ -2404,16 +2646,16 @@
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="16" t="s">
+      <c r="E47" s="18"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D48" s="1" t="s">
@@ -2442,10 +2684,10 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="19"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -2464,8 +2706,8 @@
       <c r="I49" s="3">
         <v>0.83</v>
       </c>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="15" t="s">
@@ -2839,16 +3081,16 @@
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D68" s="21" t="s">
+      <c r="D68" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E68" s="22"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="16" t="s">
+      <c r="E68" s="18"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H68" s="17"/>
-      <c r="I68" s="18"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="22"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D69" s="1" t="s">
@@ -2877,10 +3119,10 @@
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C70" s="19"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -2899,8 +3141,8 @@
       <c r="I70" s="3">
         <v>0.83</v>
       </c>
-      <c r="J70" s="20"/>
-      <c r="K70" s="20"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="15" t="s">
@@ -3264,23 +3506,37 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B13:C13"/>
@@ -3297,37 +3553,23 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3339,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC96467C-DBF9-473B-A5B5-0D1C73493020}">
   <dimension ref="B2:V150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M133" zoomScale="101" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:V150"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="101" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K151" sqref="K151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3372,26 +3614,26 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
-      <c r="O5" s="21" t="s">
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="O5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="16" t="s">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="17"/>
-      <c r="T5" s="18"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
@@ -3444,10 +3686,10 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -3466,12 +3708,12 @@
       <c r="I7" s="3">
         <v>0.83</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="M7" s="19" t="s">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="M7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="19"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -3490,11 +3732,11 @@
       <c r="T7" s="3">
         <v>0.83</v>
       </c>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -3524,7 +3766,7 @@
       <c r="K8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="23" t="s">
         <v>13</v>
       </c>
       <c r="N8" s="9" t="s">
@@ -3556,7 +3798,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="26"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="9" t="s">
         <v>99</v>
       </c>
@@ -3584,7 +3826,7 @@
       <c r="K9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M9" s="26"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="9" t="s">
         <v>99</v>
       </c>
@@ -3614,7 +3856,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="26"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="9" t="s">
         <v>100</v>
       </c>
@@ -3642,7 +3884,7 @@
       <c r="K10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M10" s="26"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="9" t="s">
         <v>100</v>
       </c>
@@ -3672,7 +3914,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="26"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="9" t="s">
         <v>101</v>
       </c>
@@ -3700,7 +3942,7 @@
       <c r="K11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M11" s="26"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="9" t="s">
         <v>101</v>
       </c>
@@ -3730,7 +3972,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="26"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="9" t="s">
         <v>102</v>
       </c>
@@ -3758,7 +4000,7 @@
       <c r="K12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M12" s="26"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="9" t="s">
         <v>102</v>
       </c>
@@ -3788,7 +4030,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="9" t="s">
         <v>103</v>
       </c>
@@ -3816,9 +4058,13 @@
         <f t="shared" si="0"/>
         <v>0.63800000000000001</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="M13" s="27"/>
+      <c r="J13" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M13" s="25"/>
       <c r="N13" s="9" t="s">
         <v>103</v>
       </c>
@@ -3846,11 +4092,15 @@
         <f t="shared" si="1"/>
         <v>0.67200000000000004</v>
       </c>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="U13" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -3880,7 +4130,7 @@
       <c r="K14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M14" s="25" t="s">
+      <c r="M14" s="23" t="s">
         <v>15</v>
       </c>
       <c r="N14" s="9" t="s">
@@ -3912,7 +4162,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="26"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="9" t="s">
         <v>99</v>
       </c>
@@ -3940,7 +4190,7 @@
       <c r="K15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="26"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="9" t="s">
         <v>99</v>
       </c>
@@ -3970,7 +4220,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="26"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="9" t="s">
         <v>100</v>
       </c>
@@ -3998,7 +4248,7 @@
       <c r="K16" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="M16" s="26"/>
+      <c r="M16" s="24"/>
       <c r="N16" s="9" t="s">
         <v>100</v>
       </c>
@@ -4028,7 +4278,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B17" s="26"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="9" t="s">
         <v>101</v>
       </c>
@@ -4056,7 +4306,7 @@
       <c r="K17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M17" s="26"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="9" t="s">
         <v>101</v>
       </c>
@@ -4086,7 +4336,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="9" t="s">
         <v>102</v>
       </c>
@@ -4114,7 +4364,7 @@
       <c r="K18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="M18" s="26"/>
+      <c r="M18" s="24"/>
       <c r="N18" s="9" t="s">
         <v>102</v>
       </c>
@@ -4144,7 +4394,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B19" s="27"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="9" t="s">
         <v>103</v>
       </c>
@@ -4172,9 +4422,13 @@
         <f t="shared" si="2"/>
         <v>0.54200000000000004</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="M19" s="27"/>
+      <c r="J19" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M19" s="25"/>
       <c r="N19" s="9" t="s">
         <v>103</v>
       </c>
@@ -4202,11 +4456,15 @@
         <f t="shared" si="3"/>
         <v>0.53200000000000003</v>
       </c>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
+      <c r="U19" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -4236,7 +4494,7 @@
       <c r="K20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="26" t="s">
         <v>16</v>
       </c>
       <c r="N20" s="9" t="s">
@@ -4268,7 +4526,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B21" s="24"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="9" t="s">
         <v>99</v>
       </c>
@@ -4296,7 +4554,7 @@
       <c r="K21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M21" s="24"/>
+      <c r="M21" s="26"/>
       <c r="N21" s="9" t="s">
         <v>99</v>
       </c>
@@ -4326,7 +4584,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="9" t="s">
         <v>100</v>
       </c>
@@ -4354,7 +4612,7 @@
       <c r="K22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="26"/>
       <c r="N22" s="9" t="s">
         <v>100</v>
       </c>
@@ -4384,7 +4642,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B23" s="24"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="9" t="s">
         <v>101</v>
       </c>
@@ -4412,7 +4670,7 @@
       <c r="K23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M23" s="24"/>
+      <c r="M23" s="26"/>
       <c r="N23" s="9" t="s">
         <v>101</v>
       </c>
@@ -4442,7 +4700,7 @@
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B24" s="24"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="9" t="s">
         <v>102</v>
       </c>
@@ -4470,7 +4728,7 @@
       <c r="K24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M24" s="24"/>
+      <c r="M24" s="26"/>
       <c r="N24" s="9" t="s">
         <v>102</v>
       </c>
@@ -4500,7 +4758,7 @@
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B25" s="24"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="9" t="s">
         <v>103</v>
       </c>
@@ -4528,9 +4786,13 @@
         <f t="shared" si="4"/>
         <v>0.54200000000000004</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="M25" s="24"/>
+      <c r="J25" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="M25" s="26"/>
       <c r="N25" s="9" t="s">
         <v>103</v>
       </c>
@@ -4558,11 +4820,15 @@
         <f t="shared" si="5"/>
         <v>0.59400000000000008</v>
       </c>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
+      <c r="U25" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -4592,7 +4858,7 @@
       <c r="K26" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M26" s="24" t="s">
+      <c r="M26" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N26" s="9" t="s">
@@ -4624,7 +4890,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B27" s="24"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="9" t="s">
         <v>99</v>
       </c>
@@ -4652,7 +4918,7 @@
       <c r="K27" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M27" s="24"/>
+      <c r="M27" s="26"/>
       <c r="N27" s="9" t="s">
         <v>99</v>
       </c>
@@ -4682,7 +4948,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B28" s="24"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="9" t="s">
         <v>100</v>
       </c>
@@ -4710,7 +4976,7 @@
       <c r="K28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="26"/>
       <c r="N28" s="9" t="s">
         <v>100</v>
       </c>
@@ -4740,7 +5006,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B29" s="24"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="9" t="s">
         <v>101</v>
       </c>
@@ -4768,7 +5034,7 @@
       <c r="K29" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M29" s="24"/>
+      <c r="M29" s="26"/>
       <c r="N29" s="9" t="s">
         <v>101</v>
       </c>
@@ -4798,7 +5064,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B30" s="24"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="9" t="s">
         <v>102</v>
       </c>
@@ -4826,7 +5092,7 @@
       <c r="K30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M30" s="24"/>
+      <c r="M30" s="26"/>
       <c r="N30" s="9" t="s">
         <v>102</v>
       </c>
@@ -4856,7 +5122,7 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B31" s="24"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="9" t="s">
         <v>103</v>
       </c>
@@ -4884,9 +5150,13 @@
         <f t="shared" si="6"/>
         <v>0.54200000000000004</v>
       </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="M31" s="24"/>
+      <c r="J31" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="M31" s="26"/>
       <c r="N31" s="9" t="s">
         <v>103</v>
       </c>
@@ -4914,11 +5184,15 @@
         <f t="shared" si="7"/>
         <v>0.55400000000000005</v>
       </c>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
+      <c r="U31" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -4948,7 +5222,7 @@
       <c r="K32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M32" s="24" t="s">
+      <c r="M32" s="26" t="s">
         <v>18</v>
       </c>
       <c r="N32" s="9" t="s">
@@ -4980,7 +5254,7 @@
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B33" s="24"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="9" t="s">
         <v>99</v>
       </c>
@@ -5008,7 +5282,7 @@
       <c r="K33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M33" s="24"/>
+      <c r="M33" s="26"/>
       <c r="N33" s="9" t="s">
         <v>99</v>
       </c>
@@ -5038,7 +5312,7 @@
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B34" s="24"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="9" t="s">
         <v>100</v>
       </c>
@@ -5066,7 +5340,7 @@
       <c r="K34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M34" s="24"/>
+      <c r="M34" s="26"/>
       <c r="N34" s="9" t="s">
         <v>100</v>
       </c>
@@ -5096,7 +5370,7 @@
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B35" s="24"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="9" t="s">
         <v>101</v>
       </c>
@@ -5124,7 +5398,7 @@
       <c r="K35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="M35" s="24"/>
+      <c r="M35" s="26"/>
       <c r="N35" s="9" t="s">
         <v>101</v>
       </c>
@@ -5154,7 +5428,7 @@
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B36" s="24"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="9" t="s">
         <v>102</v>
       </c>
@@ -5182,7 +5456,7 @@
       <c r="K36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M36" s="24"/>
+      <c r="M36" s="26"/>
       <c r="N36" s="9" t="s">
         <v>102</v>
       </c>
@@ -5212,7 +5486,7 @@
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="9" t="s">
         <v>103</v>
       </c>
@@ -5240,9 +5514,13 @@
         <f t="shared" si="8"/>
         <v>0.58200000000000007</v>
       </c>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="M37" s="24"/>
+      <c r="J37" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M37" s="26"/>
       <c r="N37" s="9" t="s">
         <v>103</v>
       </c>
@@ -5270,11 +5548,15 @@
         <f t="shared" si="9"/>
         <v>0.58599999999999997</v>
       </c>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
+      <c r="U37" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="V37" s="2" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -5304,7 +5586,7 @@
       <c r="K38" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M38" s="24" t="s">
+      <c r="M38" s="26" t="s">
         <v>19</v>
       </c>
       <c r="N38" s="9" t="s">
@@ -5336,7 +5618,7 @@
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B39" s="24"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="9" t="s">
         <v>99</v>
       </c>
@@ -5364,7 +5646,7 @@
       <c r="K39" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M39" s="24"/>
+      <c r="M39" s="26"/>
       <c r="N39" s="9" t="s">
         <v>99</v>
       </c>
@@ -5394,7 +5676,7 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B40" s="24"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="9" t="s">
         <v>100</v>
       </c>
@@ -5422,7 +5704,7 @@
       <c r="K40" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="M40" s="24"/>
+      <c r="M40" s="26"/>
       <c r="N40" s="9" t="s">
         <v>100</v>
       </c>
@@ -5452,7 +5734,7 @@
       </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B41" s="24"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="9" t="s">
         <v>101</v>
       </c>
@@ -5480,7 +5762,7 @@
       <c r="K41" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M41" s="24"/>
+      <c r="M41" s="26"/>
       <c r="N41" s="9" t="s">
         <v>101</v>
       </c>
@@ -5510,7 +5792,7 @@
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B42" s="24"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="9" t="s">
         <v>102</v>
       </c>
@@ -5538,7 +5820,7 @@
       <c r="K42" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="M42" s="24"/>
+      <c r="M42" s="26"/>
       <c r="N42" s="9" t="s">
         <v>102</v>
       </c>
@@ -5568,7 +5850,7 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B43" s="24"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="9" t="s">
         <v>103</v>
       </c>
@@ -5596,9 +5878,13 @@
         <f t="shared" si="10"/>
         <v>0.60600000000000009</v>
       </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="M43" s="24"/>
+      <c r="J43" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="M43" s="26"/>
       <c r="N43" s="9" t="s">
         <v>103</v>
       </c>
@@ -5626,11 +5912,15 @@
         <f t="shared" si="11"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
+      <c r="U43" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -5660,7 +5950,7 @@
       <c r="K44" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M44" s="24" t="s">
+      <c r="M44" s="26" t="s">
         <v>20</v>
       </c>
       <c r="N44" s="9" t="s">
@@ -5692,20 +5982,20 @@
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="13">
         <v>0.8</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="13">
         <v>0.8</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="13">
         <v>0.79</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <v>0.83</v>
       </c>
       <c r="H45" s="6">
@@ -5720,20 +6010,20 @@
       <c r="K45" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M45" s="24"/>
+      <c r="M45" s="26"/>
       <c r="N45" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="O45" s="12">
+      <c r="O45" s="11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="P45" s="12">
+      <c r="P45" s="11">
         <v>0.54</v>
       </c>
-      <c r="Q45" s="12">
+      <c r="Q45" s="11">
         <v>0.53</v>
       </c>
-      <c r="R45" s="13">
+      <c r="R45" s="12">
         <v>0.7</v>
       </c>
       <c r="S45" s="6">
@@ -5750,7 +6040,7 @@
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="9" t="s">
         <v>100</v>
       </c>
@@ -5778,7 +6068,7 @@
       <c r="K46" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="M46" s="24"/>
+      <c r="M46" s="26"/>
       <c r="N46" s="9" t="s">
         <v>100</v>
       </c>
@@ -5808,7 +6098,7 @@
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B47" s="24"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="9" t="s">
         <v>101</v>
       </c>
@@ -5836,7 +6126,7 @@
       <c r="K47" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M47" s="24"/>
+      <c r="M47" s="26"/>
       <c r="N47" s="9" t="s">
         <v>101</v>
       </c>
@@ -5866,7 +6156,7 @@
       </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B48" s="24"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="9" t="s">
         <v>102</v>
       </c>
@@ -5894,7 +6184,7 @@
       <c r="K48" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="M48" s="24"/>
+      <c r="M48" s="26"/>
       <c r="N48" s="9" t="s">
         <v>102</v>
       </c>
@@ -5924,7 +6214,7 @@
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B49" s="24"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="9" t="s">
         <v>103</v>
       </c>
@@ -5952,9 +6242,13 @@
         <f t="shared" si="12"/>
         <v>0.60600000000000009</v>
       </c>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="M49" s="24"/>
+      <c r="J49" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="M49" s="26"/>
       <c r="N49" s="9" t="s">
         <v>103</v>
       </c>
@@ -5982,11 +6276,15 @@
         <f t="shared" si="13"/>
         <v>0.55800000000000005</v>
       </c>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
+      <c r="U49" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -6016,7 +6314,7 @@
       <c r="K50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M50" s="24" t="s">
+      <c r="M50" s="26" t="s">
         <v>8</v>
       </c>
       <c r="N50" s="9" t="s">
@@ -6048,7 +6346,7 @@
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B51" s="24"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="9" t="s">
         <v>99</v>
       </c>
@@ -6076,7 +6374,7 @@
       <c r="K51" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M51" s="24"/>
+      <c r="M51" s="26"/>
       <c r="N51" s="9" t="s">
         <v>99</v>
       </c>
@@ -6106,7 +6404,7 @@
       </c>
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B52" s="24"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="9" t="s">
         <v>100</v>
       </c>
@@ -6134,7 +6432,7 @@
       <c r="K52" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M52" s="24"/>
+      <c r="M52" s="26"/>
       <c r="N52" s="9" t="s">
         <v>100</v>
       </c>
@@ -6164,7 +6462,7 @@
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B53" s="24"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="9" t="s">
         <v>101</v>
       </c>
@@ -6192,7 +6490,7 @@
       <c r="K53" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M53" s="24"/>
+      <c r="M53" s="26"/>
       <c r="N53" s="9" t="s">
         <v>101</v>
       </c>
@@ -6222,7 +6520,7 @@
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B54" s="24"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="9" t="s">
         <v>102</v>
       </c>
@@ -6250,7 +6548,7 @@
       <c r="K54" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M54" s="24"/>
+      <c r="M54" s="26"/>
       <c r="N54" s="9" t="s">
         <v>102</v>
       </c>
@@ -6280,7 +6578,7 @@
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B55" s="24"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="9" t="s">
         <v>103</v>
       </c>
@@ -6308,9 +6606,13 @@
         <f t="shared" si="14"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="M55" s="24"/>
+      <c r="J55" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="M55" s="26"/>
       <c r="N55" s="9" t="s">
         <v>103</v>
       </c>
@@ -6338,11 +6640,15 @@
         <f t="shared" si="15"/>
         <v>0.57999999999999985</v>
       </c>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
+      <c r="U55" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="V55" s="2" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -6372,7 +6678,7 @@
       <c r="K56" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M56" s="24" t="s">
+      <c r="M56" s="26" t="s">
         <v>9</v>
       </c>
       <c r="N56" s="9" t="s">
@@ -6404,7 +6710,7 @@
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B57" s="24"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="9" t="s">
         <v>99</v>
       </c>
@@ -6432,7 +6738,7 @@
       <c r="K57" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M57" s="24"/>
+      <c r="M57" s="26"/>
       <c r="N57" s="9" t="s">
         <v>99</v>
       </c>
@@ -6462,7 +6768,7 @@
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B58" s="24"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="9" t="s">
         <v>100</v>
       </c>
@@ -6490,7 +6796,7 @@
       <c r="K58" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M58" s="24"/>
+      <c r="M58" s="26"/>
       <c r="N58" s="9" t="s">
         <v>100</v>
       </c>
@@ -6520,7 +6826,7 @@
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B59" s="24"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="9" t="s">
         <v>101</v>
       </c>
@@ -6548,7 +6854,7 @@
       <c r="K59" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="M59" s="24"/>
+      <c r="M59" s="26"/>
       <c r="N59" s="9" t="s">
         <v>101</v>
       </c>
@@ -6578,7 +6884,7 @@
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B60" s="24"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="9" t="s">
         <v>102</v>
       </c>
@@ -6606,7 +6912,7 @@
       <c r="K60" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="M60" s="24"/>
+      <c r="M60" s="26"/>
       <c r="N60" s="9" t="s">
         <v>102</v>
       </c>
@@ -6636,7 +6942,7 @@
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B61" s="24"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="9" t="s">
         <v>103</v>
       </c>
@@ -6664,9 +6970,13 @@
         <f t="shared" si="16"/>
         <v>0.56399999999999995</v>
       </c>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="M61" s="24"/>
+      <c r="J61" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="M61" s="26"/>
       <c r="N61" s="9" t="s">
         <v>103</v>
       </c>
@@ -6694,11 +7004,15 @@
         <f>(T56+T57+T58+T59+T60)/5</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="U61" s="2"/>
-      <c r="V61" s="2"/>
+      <c r="U61" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="V61" s="2" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -6728,7 +7042,7 @@
       <c r="K62" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M62" s="24" t="s">
+      <c r="M62" s="26" t="s">
         <v>10</v>
       </c>
       <c r="N62" s="9" t="s">
@@ -6760,7 +7074,7 @@
       </c>
     </row>
     <row r="63" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B63" s="24"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="9" t="s">
         <v>99</v>
       </c>
@@ -6788,7 +7102,7 @@
       <c r="K63" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M63" s="24"/>
+      <c r="M63" s="26"/>
       <c r="N63" s="9" t="s">
         <v>99</v>
       </c>
@@ -6818,7 +7132,7 @@
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B64" s="24"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="9" t="s">
         <v>100</v>
       </c>
@@ -6846,7 +7160,7 @@
       <c r="K64" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M64" s="24"/>
+      <c r="M64" s="26"/>
       <c r="N64" s="9" t="s">
         <v>100</v>
       </c>
@@ -6876,7 +7190,7 @@
       </c>
     </row>
     <row r="65" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B65" s="24"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="9" t="s">
         <v>101</v>
       </c>
@@ -6904,7 +7218,7 @@
       <c r="K65" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M65" s="24"/>
+      <c r="M65" s="26"/>
       <c r="N65" s="9" t="s">
         <v>101</v>
       </c>
@@ -6934,7 +7248,7 @@
       </c>
     </row>
     <row r="66" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B66" s="24"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="9" t="s">
         <v>102</v>
       </c>
@@ -6962,7 +7276,7 @@
       <c r="K66" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M66" s="24"/>
+      <c r="M66" s="26"/>
       <c r="N66" s="9" t="s">
         <v>102</v>
       </c>
@@ -6992,7 +7306,7 @@
       </c>
     </row>
     <row r="67" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B67" s="24"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="9" t="s">
         <v>103</v>
       </c>
@@ -7020,9 +7334,13 @@
         <f t="shared" si="18"/>
         <v>0.59000000000000008</v>
       </c>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="M67" s="24"/>
+      <c r="J67" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="M67" s="26"/>
       <c r="N67" s="9" t="s">
         <v>103</v>
       </c>
@@ -7050,11 +7368,15 @@
         <f t="shared" si="19"/>
         <v>0.61599999999999999</v>
       </c>
-      <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
+      <c r="U67" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="V67" s="2" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="68" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="9" t="s">
@@ -7084,7 +7406,7 @@
       <c r="K68" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M68" s="24" t="s">
+      <c r="M68" s="26" t="s">
         <v>11</v>
       </c>
       <c r="N68" s="9" t="s">
@@ -7116,7 +7438,7 @@
       </c>
     </row>
     <row r="69" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B69" s="24"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="9" t="s">
         <v>99</v>
       </c>
@@ -7144,7 +7466,7 @@
       <c r="K69" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M69" s="24"/>
+      <c r="M69" s="26"/>
       <c r="N69" s="9" t="s">
         <v>99</v>
       </c>
@@ -7174,7 +7496,7 @@
       </c>
     </row>
     <row r="70" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B70" s="24"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="9" t="s">
         <v>100</v>
       </c>
@@ -7202,7 +7524,7 @@
       <c r="K70" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M70" s="24"/>
+      <c r="M70" s="26"/>
       <c r="N70" s="9" t="s">
         <v>100</v>
       </c>
@@ -7232,7 +7554,7 @@
       </c>
     </row>
     <row r="71" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B71" s="24"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="9" t="s">
         <v>101</v>
       </c>
@@ -7260,7 +7582,7 @@
       <c r="K71" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M71" s="24"/>
+      <c r="M71" s="26"/>
       <c r="N71" s="9" t="s">
         <v>101</v>
       </c>
@@ -7290,7 +7612,7 @@
       </c>
     </row>
     <row r="72" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B72" s="24"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="9" t="s">
         <v>102</v>
       </c>
@@ -7318,7 +7640,7 @@
       <c r="K72" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="M72" s="24"/>
+      <c r="M72" s="26"/>
       <c r="N72" s="9" t="s">
         <v>102</v>
       </c>
@@ -7348,7 +7670,7 @@
       </c>
     </row>
     <row r="73" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B73" s="24"/>
+      <c r="B73" s="26"/>
       <c r="C73" s="9" t="s">
         <v>103</v>
       </c>
@@ -7376,9 +7698,13 @@
         <f t="shared" si="20"/>
         <v>0.61599999999999999</v>
       </c>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="M73" s="24"/>
+      <c r="J73" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M73" s="26"/>
       <c r="N73" s="9" t="s">
         <v>103</v>
       </c>
@@ -7406,8 +7732,12 @@
         <f t="shared" si="21"/>
         <v>0.64200000000000002</v>
       </c>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
+      <c r="U73" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="V73" s="2" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="79" spans="2:22" ht="21" x14ac:dyDescent="0.4">
       <c r="B79" s="4" t="s">
@@ -7428,26 +7758,26 @@
       </c>
     </row>
     <row r="82" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D82" s="21" t="s">
+      <c r="D82" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E82" s="22"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="16" t="s">
+      <c r="E82" s="18"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H82" s="17"/>
-      <c r="I82" s="18"/>
-      <c r="O82" s="21" t="s">
+      <c r="H82" s="21"/>
+      <c r="I82" s="22"/>
+      <c r="O82" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="P82" s="22"/>
-      <c r="Q82" s="23"/>
-      <c r="R82" s="16" t="s">
+      <c r="P82" s="18"/>
+      <c r="Q82" s="19"/>
+      <c r="R82" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="S82" s="17"/>
-      <c r="T82" s="18"/>
+      <c r="S82" s="21"/>
+      <c r="T82" s="22"/>
     </row>
     <row r="83" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D83" s="1" t="s">
@@ -7500,10 +7830,10 @@
       </c>
     </row>
     <row r="84" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B84" s="19" t="s">
+      <c r="B84" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C84" s="19"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -7522,12 +7852,12 @@
       <c r="I84" s="3">
         <v>0.83</v>
       </c>
-      <c r="J84" s="20"/>
-      <c r="K84" s="20"/>
-      <c r="M84" s="19" t="s">
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="M84" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N84" s="19"/>
+      <c r="N84" s="16"/>
       <c r="O84" s="3">
         <v>0.75529999999999997</v>
       </c>
@@ -7546,11 +7876,11 @@
       <c r="T84" s="3">
         <v>0.83</v>
       </c>
-      <c r="U84" s="20"/>
-      <c r="V84" s="20"/>
+      <c r="U84" s="14"/>
+      <c r="V84" s="14"/>
     </row>
     <row r="85" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B85" s="25" t="s">
+      <c r="B85" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="9" t="s">
@@ -7580,7 +7910,7 @@
       <c r="K85" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="M85" s="25" t="s">
+      <c r="M85" s="23" t="s">
         <v>13</v>
       </c>
       <c r="N85" s="9" t="s">
@@ -7612,7 +7942,7 @@
       </c>
     </row>
     <row r="86" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B86" s="26"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="9" t="s">
         <v>99</v>
       </c>
@@ -7640,7 +7970,7 @@
       <c r="K86" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="M86" s="26"/>
+      <c r="M86" s="24"/>
       <c r="N86" s="9" t="s">
         <v>99</v>
       </c>
@@ -7670,7 +8000,7 @@
       </c>
     </row>
     <row r="87" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B87" s="26"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="9" t="s">
         <v>100</v>
       </c>
@@ -7698,7 +8028,7 @@
       <c r="K87" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M87" s="26"/>
+      <c r="M87" s="24"/>
       <c r="N87" s="9" t="s">
         <v>100</v>
       </c>
@@ -7721,14 +8051,14 @@
         <v>0.67</v>
       </c>
       <c r="U87" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V87" s="2" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="88" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B88" s="26"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="9" t="s">
         <v>101</v>
       </c>
@@ -7756,7 +8086,7 @@
       <c r="K88" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M88" s="26"/>
+      <c r="M88" s="24"/>
       <c r="N88" s="9" t="s">
         <v>101</v>
       </c>
@@ -7786,7 +8116,7 @@
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B89" s="26"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="9" t="s">
         <v>102</v>
       </c>
@@ -7814,7 +8144,7 @@
       <c r="K89" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="M89" s="26"/>
+      <c r="M89" s="24"/>
       <c r="N89" s="9" t="s">
         <v>102</v>
       </c>
@@ -7840,11 +8170,11 @@
         <v>223</v>
       </c>
       <c r="V89" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B90" s="27"/>
+      <c r="B90" s="25"/>
       <c r="C90" s="9" t="s">
         <v>103</v>
       </c>
@@ -7872,9 +8202,13 @@
         <f t="shared" si="22"/>
         <v>0.58000000000000007</v>
       </c>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="M90" s="27"/>
+      <c r="J90" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="M90" s="25"/>
       <c r="N90" s="9" t="s">
         <v>103</v>
       </c>
@@ -7902,11 +8236,15 @@
         <f t="shared" ref="T90" si="28">(T85+T86+T87+T88+T89)/5</f>
         <v>0.59000000000000008</v>
       </c>
-      <c r="U90" s="2"/>
-      <c r="V90" s="2"/>
+      <c r="U90" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="V90" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B91" s="25" t="s">
+      <c r="B91" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C91" s="9" t="s">
@@ -7936,7 +8274,7 @@
       <c r="K91" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M91" s="25" t="s">
+      <c r="M91" s="23" t="s">
         <v>15</v>
       </c>
       <c r="N91" s="9" t="s">
@@ -7968,7 +8306,7 @@
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B92" s="26"/>
+      <c r="B92" s="24"/>
       <c r="C92" s="9" t="s">
         <v>99</v>
       </c>
@@ -7996,7 +8334,7 @@
       <c r="K92" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="M92" s="26"/>
+      <c r="M92" s="24"/>
       <c r="N92" s="9" t="s">
         <v>99</v>
       </c>
@@ -8026,7 +8364,7 @@
       </c>
     </row>
     <row r="93" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B93" s="26"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="9" t="s">
         <v>100</v>
       </c>
@@ -8054,7 +8392,7 @@
       <c r="K93" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="M93" s="26"/>
+      <c r="M93" s="24"/>
       <c r="N93" s="9" t="s">
         <v>100</v>
       </c>
@@ -8077,14 +8415,14 @@
         <v>0.6</v>
       </c>
       <c r="U93" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="V93" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="V93" s="8" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="94" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B94" s="26"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="9" t="s">
         <v>101</v>
       </c>
@@ -8112,7 +8450,7 @@
       <c r="K94" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M94" s="26"/>
+      <c r="M94" s="24"/>
       <c r="N94" s="9" t="s">
         <v>101</v>
       </c>
@@ -8135,14 +8473,14 @@
         <v>0.5</v>
       </c>
       <c r="U94" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V94" s="2" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="95" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B95" s="26"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="9" t="s">
         <v>102</v>
       </c>
@@ -8170,7 +8508,7 @@
       <c r="K95" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="M95" s="26"/>
+      <c r="M95" s="24"/>
       <c r="N95" s="9" t="s">
         <v>102</v>
       </c>
@@ -8193,14 +8531,14 @@
         <v>0.45</v>
       </c>
       <c r="U95" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="V95" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="V95" s="2" t="s">
-        <v>284</v>
-      </c>
     </row>
     <row r="96" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B96" s="27"/>
+      <c r="B96" s="25"/>
       <c r="C96" s="9" t="s">
         <v>103</v>
       </c>
@@ -8228,9 +8566,13 @@
         <f t="shared" si="29"/>
         <v>0.57400000000000007</v>
       </c>
-      <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
-      <c r="M96" s="27"/>
+      <c r="J96" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M96" s="25"/>
       <c r="N96" s="9" t="s">
         <v>103</v>
       </c>
@@ -8258,11 +8600,15 @@
         <f t="shared" ref="T96" si="35">(T91+T92+T93+T94+T95)/5</f>
         <v>0.54400000000000004</v>
       </c>
-      <c r="U96" s="2"/>
-      <c r="V96" s="2"/>
+      <c r="U96" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="V96" s="2" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="97" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B97" s="24" t="s">
+      <c r="B97" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C97" s="9" t="s">
@@ -8292,7 +8638,7 @@
       <c r="K97" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M97" s="24" t="s">
+      <c r="M97" s="26" t="s">
         <v>16</v>
       </c>
       <c r="N97" s="9" t="s">
@@ -8324,7 +8670,7 @@
       </c>
     </row>
     <row r="98" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B98" s="24"/>
+      <c r="B98" s="26"/>
       <c r="C98" s="9" t="s">
         <v>99</v>
       </c>
@@ -8352,7 +8698,7 @@
       <c r="K98" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M98" s="24"/>
+      <c r="M98" s="26"/>
       <c r="N98" s="9" t="s">
         <v>99</v>
       </c>
@@ -8382,7 +8728,7 @@
       </c>
     </row>
     <row r="99" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B99" s="24"/>
+      <c r="B99" s="26"/>
       <c r="C99" s="9" t="s">
         <v>100</v>
       </c>
@@ -8410,7 +8756,7 @@
       <c r="K99" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="M99" s="24"/>
+      <c r="M99" s="26"/>
       <c r="N99" s="9" t="s">
         <v>100</v>
       </c>
@@ -8433,14 +8779,14 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="U99" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V99" s="2" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="100" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B100" s="24"/>
+      <c r="B100" s="26"/>
       <c r="C100" s="9" t="s">
         <v>101</v>
       </c>
@@ -8468,7 +8814,7 @@
       <c r="K100" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M100" s="24"/>
+      <c r="M100" s="26"/>
       <c r="N100" s="9" t="s">
         <v>101</v>
       </c>
@@ -8491,14 +8837,14 @@
         <v>0.6</v>
       </c>
       <c r="U100" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V100" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B101" s="24"/>
+      <c r="B101" s="26"/>
       <c r="C101" s="9" t="s">
         <v>102</v>
       </c>
@@ -8524,9 +8870,9 @@
         <v>125</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="M101" s="24"/>
+        <v>370</v>
+      </c>
+      <c r="M101" s="26"/>
       <c r="N101" s="9" t="s">
         <v>102</v>
       </c>
@@ -8552,11 +8898,11 @@
         <v>237</v>
       </c>
       <c r="V101" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B102" s="24"/>
+      <c r="B102" s="26"/>
       <c r="C102" s="9" t="s">
         <v>103</v>
       </c>
@@ -8584,9 +8930,13 @@
         <f t="shared" si="36"/>
         <v>0.55199999999999994</v>
       </c>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="M102" s="24"/>
+      <c r="J102" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="M102" s="26"/>
       <c r="N102" s="9" t="s">
         <v>103</v>
       </c>
@@ -8614,11 +8964,15 @@
         <f t="shared" ref="T102" si="42">(T97+T98+T99+T100+T101)/5</f>
         <v>0.52200000000000002</v>
       </c>
-      <c r="U102" s="11"/>
-      <c r="V102" s="11"/>
+      <c r="U102" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="V102" s="2" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="103" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C103" s="9" t="s">
@@ -8648,7 +9002,7 @@
       <c r="K103" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M103" s="24" t="s">
+      <c r="M103" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N103" s="9" t="s">
@@ -8680,7 +9034,7 @@
       </c>
     </row>
     <row r="104" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B104" s="24"/>
+      <c r="B104" s="26"/>
       <c r="C104" s="9" t="s">
         <v>99</v>
       </c>
@@ -8708,7 +9062,7 @@
       <c r="K104" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M104" s="24"/>
+      <c r="M104" s="26"/>
       <c r="N104" s="9" t="s">
         <v>99</v>
       </c>
@@ -8738,7 +9092,7 @@
       </c>
     </row>
     <row r="105" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B105" s="24"/>
+      <c r="B105" s="26"/>
       <c r="C105" s="9" t="s">
         <v>100</v>
       </c>
@@ -8761,12 +9115,12 @@
         <v>0.63</v>
       </c>
       <c r="J105" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K105" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K105" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="M105" s="24"/>
+      <c r="M105" s="26"/>
       <c r="N105" s="9" t="s">
         <v>100</v>
       </c>
@@ -8789,14 +9143,14 @@
         <v>0.7</v>
       </c>
       <c r="U105" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V105" s="2" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="106" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B106" s="24"/>
+      <c r="B106" s="26"/>
       <c r="C106" s="9" t="s">
         <v>101</v>
       </c>
@@ -8822,9 +9176,9 @@
         <v>153</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M106" s="24"/>
+        <v>256</v>
+      </c>
+      <c r="M106" s="26"/>
       <c r="N106" s="9" t="s">
         <v>101</v>
       </c>
@@ -8847,14 +9201,14 @@
         <v>0.63</v>
       </c>
       <c r="U106" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="V106" s="2" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="107" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B107" s="24"/>
+      <c r="B107" s="26"/>
       <c r="C107" s="9" t="s">
         <v>102</v>
       </c>
@@ -8877,12 +9231,12 @@
         <v>0.5</v>
       </c>
       <c r="J107" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K107" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="K107" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="M107" s="24"/>
+      <c r="M107" s="26"/>
       <c r="N107" s="9" t="s">
         <v>102</v>
       </c>
@@ -8905,14 +9259,14 @@
         <v>0.65</v>
       </c>
       <c r="U107" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="V107" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="108" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B108" s="24"/>
+      <c r="B108" s="26"/>
       <c r="C108" s="9" t="s">
         <v>103</v>
       </c>
@@ -8940,9 +9294,13 @@
         <f t="shared" si="43"/>
         <v>0.59399999999999997</v>
       </c>
-      <c r="J108" s="11"/>
-      <c r="K108" s="11"/>
-      <c r="M108" s="24"/>
+      <c r="J108" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="M108" s="26"/>
       <c r="N108" s="9" t="s">
         <v>103</v>
       </c>
@@ -8970,11 +9328,15 @@
         <f t="shared" ref="T108" si="49">(T103+T104+T105+T106+T107)/5</f>
         <v>0.622</v>
       </c>
-      <c r="U108" s="11"/>
-      <c r="V108" s="11"/>
+      <c r="U108" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="V108" s="2" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="109" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B109" s="24" t="s">
+      <c r="B109" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C109" s="9" t="s">
@@ -8999,12 +9361,12 @@
         <v>0.44</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M109" s="24" t="s">
+      <c r="M109" s="26" t="s">
         <v>18</v>
       </c>
       <c r="N109" s="9" t="s">
@@ -9036,7 +9398,7 @@
       </c>
     </row>
     <row r="110" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B110" s="24"/>
+      <c r="B110" s="26"/>
       <c r="C110" s="9" t="s">
         <v>99</v>
       </c>
@@ -9064,7 +9426,7 @@
       <c r="K110" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M110" s="24"/>
+      <c r="M110" s="26"/>
       <c r="N110" s="9" t="s">
         <v>99</v>
       </c>
@@ -9087,14 +9449,14 @@
         <v>0.73</v>
       </c>
       <c r="U110" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="V110" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="111" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B111" s="24"/>
+      <c r="B111" s="26"/>
       <c r="C111" s="9" t="s">
         <v>100</v>
       </c>
@@ -9122,7 +9484,7 @@
       <c r="K111" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M111" s="24"/>
+      <c r="M111" s="26"/>
       <c r="N111" s="9" t="s">
         <v>100</v>
       </c>
@@ -9148,11 +9510,11 @@
         <v>182</v>
       </c>
       <c r="V111" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="112" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B112" s="24"/>
+      <c r="B112" s="26"/>
       <c r="C112" s="9" t="s">
         <v>101</v>
       </c>
@@ -9175,12 +9537,12 @@
         <v>0.6</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M112" s="24"/>
+      <c r="M112" s="26"/>
       <c r="N112" s="9" t="s">
         <v>101</v>
       </c>
@@ -9203,14 +9565,14 @@
         <v>0.5</v>
       </c>
       <c r="U112" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V112" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="113" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B113" s="24"/>
+      <c r="B113" s="26"/>
       <c r="C113" s="9" t="s">
         <v>102</v>
       </c>
@@ -9233,12 +9595,12 @@
         <v>0.5</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M113" s="24"/>
+      <c r="M113" s="26"/>
       <c r="N113" s="9" t="s">
         <v>102</v>
       </c>
@@ -9261,14 +9623,14 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="U113" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="V113" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="V113" s="2" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="114" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B114" s="24"/>
+      <c r="B114" s="26"/>
       <c r="C114" s="9" t="s">
         <v>103</v>
       </c>
@@ -9296,9 +9658,13 @@
         <f t="shared" si="50"/>
         <v>0.60599999999999998</v>
       </c>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-      <c r="M114" s="24"/>
+      <c r="J114" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="M114" s="26"/>
       <c r="N114" s="9" t="s">
         <v>103</v>
       </c>
@@ -9326,11 +9692,15 @@
         <f t="shared" ref="T114" si="56">(T109+T110+T111+T112+T113)/5</f>
         <v>0.57800000000000007</v>
       </c>
-      <c r="U114" s="2"/>
-      <c r="V114" s="2"/>
+      <c r="U114" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="V114" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="115" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B115" s="24" t="s">
+      <c r="B115" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C115" s="9" t="s">
@@ -9360,7 +9730,7 @@
       <c r="K115" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M115" s="24" t="s">
+      <c r="M115" s="26" t="s">
         <v>19</v>
       </c>
       <c r="N115" s="9" t="s">
@@ -9392,7 +9762,7 @@
       </c>
     </row>
     <row r="116" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B116" s="24"/>
+      <c r="B116" s="26"/>
       <c r="C116" s="9" t="s">
         <v>99</v>
       </c>
@@ -9415,12 +9785,12 @@
         <v>0.77</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M116" s="24"/>
+      <c r="M116" s="26"/>
       <c r="N116" s="9" t="s">
         <v>99</v>
       </c>
@@ -9450,7 +9820,7 @@
       </c>
     </row>
     <row r="117" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B117" s="24"/>
+      <c r="B117" s="26"/>
       <c r="C117" s="9" t="s">
         <v>100</v>
       </c>
@@ -9478,7 +9848,7 @@
       <c r="K117" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="M117" s="24"/>
+      <c r="M117" s="26"/>
       <c r="N117" s="9" t="s">
         <v>100</v>
       </c>
@@ -9508,7 +9878,7 @@
       </c>
     </row>
     <row r="118" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B118" s="24"/>
+      <c r="B118" s="26"/>
       <c r="C118" s="9" t="s">
         <v>101</v>
       </c>
@@ -9531,12 +9901,12 @@
         <v>0.47</v>
       </c>
       <c r="J118" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="K118" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="K118" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="M118" s="24"/>
+      <c r="M118" s="26"/>
       <c r="N118" s="9" t="s">
         <v>101</v>
       </c>
@@ -9566,7 +9936,7 @@
       </c>
     </row>
     <row r="119" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B119" s="24"/>
+      <c r="B119" s="26"/>
       <c r="C119" s="9" t="s">
         <v>102</v>
       </c>
@@ -9589,12 +9959,12 @@
         <v>0.44</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M119" s="24"/>
+      <c r="M119" s="26"/>
       <c r="N119" s="9" t="s">
         <v>102</v>
       </c>
@@ -9617,14 +9987,14 @@
         <v>0.5</v>
       </c>
       <c r="U119" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="V119" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="V119" s="2" t="s">
-        <v>294</v>
-      </c>
     </row>
     <row r="120" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B120" s="24"/>
+      <c r="B120" s="26"/>
       <c r="C120" s="9" t="s">
         <v>103</v>
       </c>
@@ -9652,9 +10022,13 @@
         <f t="shared" si="57"/>
         <v>0.59</v>
       </c>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-      <c r="M120" s="24"/>
+      <c r="J120" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="M120" s="26"/>
       <c r="N120" s="9" t="s">
         <v>103</v>
       </c>
@@ -9682,11 +10056,15 @@
         <f t="shared" ref="T120" si="63">(T115+T116+T117+T118+T119)/5</f>
         <v>0.56799999999999995</v>
       </c>
-      <c r="U120" s="2"/>
-      <c r="V120" s="2"/>
+      <c r="U120" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="V120" s="2" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="121" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B121" s="24" t="s">
+      <c r="B121" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C121" s="9" t="s">
@@ -9711,12 +10089,12 @@
         <v>0.44</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K121" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M121" s="24" t="s">
+      <c r="M121" s="26" t="s">
         <v>20</v>
       </c>
       <c r="N121" s="9" t="s">
@@ -9748,20 +10126,20 @@
       </c>
     </row>
     <row r="122" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B122" s="24"/>
+      <c r="B122" s="26"/>
       <c r="C122" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D122" s="12">
+      <c r="D122" s="11">
         <v>0.47</v>
       </c>
-      <c r="E122" s="12">
+      <c r="E122" s="11">
         <v>0.47</v>
       </c>
-      <c r="F122" s="12">
+      <c r="F122" s="11">
         <v>0.47</v>
       </c>
-      <c r="G122" s="13">
+      <c r="G122" s="12">
         <v>0.78</v>
       </c>
       <c r="H122" s="6">
@@ -9776,20 +10154,20 @@
       <c r="K122" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M122" s="24"/>
+      <c r="M122" s="26"/>
       <c r="N122" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="O122" s="12">
+      <c r="O122" s="11">
         <v>0.53</v>
       </c>
-      <c r="P122" s="12">
+      <c r="P122" s="11">
         <v>0.52</v>
       </c>
-      <c r="Q122" s="12">
+      <c r="Q122" s="11">
         <v>0.5</v>
       </c>
-      <c r="R122" s="13">
+      <c r="R122" s="12">
         <v>0.75</v>
       </c>
       <c r="S122" s="6">
@@ -9799,14 +10177,14 @@
         <v>0.5</v>
       </c>
       <c r="U122" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="V122" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="123" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B123" s="24"/>
+      <c r="B123" s="26"/>
       <c r="C123" s="9" t="s">
         <v>100</v>
       </c>
@@ -9832,9 +10210,9 @@
         <v>127</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="M123" s="24"/>
+        <v>267</v>
+      </c>
+      <c r="M123" s="26"/>
       <c r="N123" s="9" t="s">
         <v>100</v>
       </c>
@@ -9857,14 +10235,14 @@
         <v>0.7</v>
       </c>
       <c r="U123" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V123" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="124" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B124" s="24"/>
+      <c r="B124" s="26"/>
       <c r="C124" s="9" t="s">
         <v>101</v>
       </c>
@@ -9887,12 +10265,12 @@
         <v>0.35</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M124" s="24"/>
+      <c r="M124" s="26"/>
       <c r="N124" s="9" t="s">
         <v>101</v>
       </c>
@@ -9922,7 +10300,7 @@
       </c>
     </row>
     <row r="125" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B125" s="24"/>
+      <c r="B125" s="26"/>
       <c r="C125" s="9" t="s">
         <v>102</v>
       </c>
@@ -9945,12 +10323,12 @@
         <v>0.65</v>
       </c>
       <c r="J125" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="K125" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="K125" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="M125" s="24"/>
+      <c r="M125" s="26"/>
       <c r="N125" s="9" t="s">
         <v>102</v>
       </c>
@@ -9980,7 +10358,7 @@
       </c>
     </row>
     <row r="126" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B126" s="24"/>
+      <c r="B126" s="26"/>
       <c r="C126" s="9" t="s">
         <v>103</v>
       </c>
@@ -10008,9 +10386,13 @@
         <f t="shared" si="64"/>
         <v>0.51400000000000001</v>
       </c>
-      <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
-      <c r="M126" s="24"/>
+      <c r="J126" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M126" s="26"/>
       <c r="N126" s="9" t="s">
         <v>103</v>
       </c>
@@ -10038,11 +10420,15 @@
         <f t="shared" ref="T126" si="70">(T121+T122+T123+T124+T125)/5</f>
         <v>0.56199999999999994</v>
       </c>
-      <c r="U126" s="2"/>
-      <c r="V126" s="2"/>
+      <c r="U126" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="V126" s="2" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="127" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B127" s="24" t="s">
+      <c r="B127" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C127" s="9" t="s">
@@ -10072,7 +10458,7 @@
       <c r="K127" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M127" s="24" t="s">
+      <c r="M127" s="26" t="s">
         <v>8</v>
       </c>
       <c r="N127" s="9" t="s">
@@ -10104,7 +10490,7 @@
       </c>
     </row>
     <row r="128" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B128" s="24"/>
+      <c r="B128" s="26"/>
       <c r="C128" s="9" t="s">
         <v>99</v>
       </c>
@@ -10132,7 +10518,7 @@
       <c r="K128" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M128" s="24"/>
+      <c r="M128" s="26"/>
       <c r="N128" s="9" t="s">
         <v>99</v>
       </c>
@@ -10155,14 +10541,14 @@
         <v>0.5</v>
       </c>
       <c r="U128" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="V128" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="129" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B129" s="24"/>
+      <c r="B129" s="26"/>
       <c r="C129" s="9" t="s">
         <v>100</v>
       </c>
@@ -10190,7 +10576,7 @@
       <c r="K129" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="M129" s="24"/>
+      <c r="M129" s="26"/>
       <c r="N129" s="9" t="s">
         <v>100</v>
       </c>
@@ -10213,14 +10599,14 @@
         <v>0.5</v>
       </c>
       <c r="U129" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="V129" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="130" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B130" s="24"/>
+      <c r="B130" s="26"/>
       <c r="C130" s="9" t="s">
         <v>101</v>
       </c>
@@ -10243,12 +10629,12 @@
         <v>0.47</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K130" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M130" s="24"/>
+      <c r="M130" s="26"/>
       <c r="N130" s="9" t="s">
         <v>101</v>
       </c>
@@ -10278,7 +10664,7 @@
       </c>
     </row>
     <row r="131" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B131" s="24"/>
+      <c r="B131" s="26"/>
       <c r="C131" s="9" t="s">
         <v>102</v>
       </c>
@@ -10301,12 +10687,12 @@
         <v>0.5</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M131" s="24"/>
+      <c r="M131" s="26"/>
       <c r="N131" s="9" t="s">
         <v>102</v>
       </c>
@@ -10329,14 +10715,14 @@
         <v>0.36</v>
       </c>
       <c r="U131" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="V131" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="V131" s="2" t="s">
-        <v>298</v>
-      </c>
     </row>
     <row r="132" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B132" s="24"/>
+      <c r="B132" s="26"/>
       <c r="C132" s="9" t="s">
         <v>103</v>
       </c>
@@ -10364,9 +10750,13 @@
         <f t="shared" si="71"/>
         <v>0.54200000000000004</v>
       </c>
-      <c r="J132" s="2"/>
-      <c r="K132" s="2"/>
-      <c r="M132" s="24"/>
+      <c r="J132" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="M132" s="26"/>
       <c r="N132" s="9" t="s">
         <v>103</v>
       </c>
@@ -10394,11 +10784,15 @@
         <f t="shared" ref="T132" si="77">(T127+T128+T129+T130+T131)/5</f>
         <v>0.49799999999999994</v>
       </c>
-      <c r="U132" s="2"/>
-      <c r="V132" s="2"/>
+      <c r="U132" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="V132" s="2" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="133" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B133" s="24" t="s">
+      <c r="B133" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C133" s="9" t="s">
@@ -10428,7 +10822,7 @@
       <c r="K133" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M133" s="24" t="s">
+      <c r="M133" s="26" t="s">
         <v>9</v>
       </c>
       <c r="N133" s="9" t="s">
@@ -10460,7 +10854,7 @@
       </c>
     </row>
     <row r="134" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B134" s="24"/>
+      <c r="B134" s="26"/>
       <c r="C134" s="9" t="s">
         <v>99</v>
       </c>
@@ -10488,7 +10882,7 @@
       <c r="K134" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M134" s="24"/>
+      <c r="M134" s="26"/>
       <c r="N134" s="9" t="s">
         <v>99</v>
       </c>
@@ -10511,14 +10905,14 @@
         <v>0.63</v>
       </c>
       <c r="U134" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V134" s="2" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="135" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B135" s="24"/>
+      <c r="B135" s="26"/>
       <c r="C135" s="9" t="s">
         <v>100</v>
       </c>
@@ -10544,9 +10938,9 @@
         <v>166</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M135" s="24"/>
+        <v>256</v>
+      </c>
+      <c r="M135" s="26"/>
       <c r="N135" s="9" t="s">
         <v>100</v>
       </c>
@@ -10576,7 +10970,7 @@
       </c>
     </row>
     <row r="136" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B136" s="24"/>
+      <c r="B136" s="26"/>
       <c r="C136" s="9" t="s">
         <v>101</v>
       </c>
@@ -10602,9 +10996,9 @@
         <v>94</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="M136" s="24"/>
+        <v>272</v>
+      </c>
+      <c r="M136" s="26"/>
       <c r="N136" s="9" t="s">
         <v>101</v>
       </c>
@@ -10627,14 +11021,14 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="U136" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V136" s="2" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="137" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B137" s="24"/>
+      <c r="B137" s="26"/>
       <c r="C137" s="9" t="s">
         <v>102</v>
       </c>
@@ -10657,12 +11051,12 @@
         <v>0.43</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K137" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M137" s="24"/>
+      <c r="M137" s="26"/>
       <c r="N137" s="9" t="s">
         <v>102</v>
       </c>
@@ -10688,11 +11082,11 @@
         <v>232</v>
       </c>
       <c r="V137" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="138" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B138" s="24"/>
+      <c r="B138" s="26"/>
       <c r="C138" s="9" t="s">
         <v>103</v>
       </c>
@@ -10720,9 +11114,13 @@
         <f t="shared" si="78"/>
         <v>0.51400000000000001</v>
       </c>
-      <c r="J138" s="2"/>
-      <c r="K138" s="2"/>
-      <c r="M138" s="24"/>
+      <c r="J138" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="K138" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="M138" s="26"/>
       <c r="N138" s="9" t="s">
         <v>103</v>
       </c>
@@ -10750,11 +11148,15 @@
         <f t="shared" ref="T138" si="84">(T133+T134+T135+T136+T137)/5</f>
         <v>0.59199999999999997</v>
       </c>
-      <c r="U138" s="2"/>
-      <c r="V138" s="2"/>
+      <c r="U138" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="V138" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="139" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B139" s="24" t="s">
+      <c r="B139" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C139" s="9" t="s">
@@ -10784,7 +11186,7 @@
       <c r="K139" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M139" s="24" t="s">
+      <c r="M139" s="26" t="s">
         <v>10</v>
       </c>
       <c r="N139" s="9" t="s">
@@ -10816,7 +11218,7 @@
       </c>
     </row>
     <row r="140" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B140" s="24"/>
+      <c r="B140" s="26"/>
       <c r="C140" s="9" t="s">
         <v>99</v>
       </c>
@@ -10839,12 +11241,12 @@
         <v>0.74</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M140" s="24"/>
+      <c r="M140" s="26"/>
       <c r="N140" s="9" t="s">
         <v>99</v>
       </c>
@@ -10874,7 +11276,7 @@
       </c>
     </row>
     <row r="141" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B141" s="24"/>
+      <c r="B141" s="26"/>
       <c r="C141" s="9" t="s">
         <v>100</v>
       </c>
@@ -10902,7 +11304,7 @@
       <c r="K141" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M141" s="24"/>
+      <c r="M141" s="26"/>
       <c r="N141" s="9" t="s">
         <v>100</v>
       </c>
@@ -10925,14 +11327,14 @@
         <v>0.67</v>
       </c>
       <c r="U141" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V141" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="142" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B142" s="24"/>
+      <c r="B142" s="26"/>
       <c r="C142" s="9" t="s">
         <v>101</v>
       </c>
@@ -10955,12 +11357,12 @@
         <v>0.6</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M142" s="24"/>
+      <c r="M142" s="26"/>
       <c r="N142" s="9" t="s">
         <v>101</v>
       </c>
@@ -10990,7 +11392,7 @@
       </c>
     </row>
     <row r="143" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B143" s="24"/>
+      <c r="B143" s="26"/>
       <c r="C143" s="9" t="s">
         <v>102</v>
       </c>
@@ -11018,7 +11420,7 @@
       <c r="K143" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M143" s="24"/>
+      <c r="M143" s="26"/>
       <c r="N143" s="9" t="s">
         <v>102</v>
       </c>
@@ -11044,11 +11446,11 @@
         <v>206</v>
       </c>
       <c r="V143" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="144" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B144" s="24"/>
+      <c r="B144" s="26"/>
       <c r="C144" s="9" t="s">
         <v>103</v>
       </c>
@@ -11076,9 +11478,13 @@
         <f t="shared" si="85"/>
         <v>0.59400000000000008</v>
       </c>
-      <c r="J144" s="2"/>
-      <c r="K144" s="2"/>
-      <c r="M144" s="24"/>
+      <c r="J144" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="K144" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="M144" s="26"/>
       <c r="N144" s="9" t="s">
         <v>103</v>
       </c>
@@ -11106,11 +11512,15 @@
         <f t="shared" ref="T144" si="91">(T139+T140+T141+T142+T143)/5</f>
         <v>0.64800000000000002</v>
       </c>
-      <c r="U144" s="2"/>
-      <c r="V144" s="2"/>
+      <c r="U144" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="V144" s="2" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="145" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B145" s="24" t="s">
+      <c r="B145" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C145" s="9" t="s">
@@ -11140,7 +11550,7 @@
       <c r="K145" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M145" s="24" t="s">
+      <c r="M145" s="26" t="s">
         <v>11</v>
       </c>
       <c r="N145" s="9" t="s">
@@ -11172,7 +11582,7 @@
       </c>
     </row>
     <row r="146" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B146" s="24"/>
+      <c r="B146" s="26"/>
       <c r="C146" s="9" t="s">
         <v>99</v>
       </c>
@@ -11195,12 +11605,12 @@
         <v>0.71</v>
       </c>
       <c r="J146" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K146" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="K146" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="M146" s="24"/>
+      <c r="M146" s="26"/>
       <c r="N146" s="9" t="s">
         <v>99</v>
       </c>
@@ -11226,11 +11636,11 @@
         <v>182</v>
       </c>
       <c r="V146" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="147" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B147" s="24"/>
+      <c r="B147" s="26"/>
       <c r="C147" s="9" t="s">
         <v>100</v>
       </c>
@@ -11258,7 +11668,7 @@
       <c r="K147" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M147" s="24"/>
+      <c r="M147" s="26"/>
       <c r="N147" s="9" t="s">
         <v>100</v>
       </c>
@@ -11284,11 +11694,11 @@
         <v>220</v>
       </c>
       <c r="V147" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="148" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B148" s="24"/>
+      <c r="B148" s="26"/>
       <c r="C148" s="9" t="s">
         <v>101</v>
       </c>
@@ -11316,7 +11726,7 @@
       <c r="K148" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M148" s="24"/>
+      <c r="M148" s="26"/>
       <c r="N148" s="9" t="s">
         <v>101</v>
       </c>
@@ -11342,11 +11752,11 @@
         <v>235</v>
       </c>
       <c r="V148" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B149" s="24"/>
+      <c r="B149" s="26"/>
       <c r="C149" s="9" t="s">
         <v>102</v>
       </c>
@@ -11369,12 +11779,12 @@
         <v>0.59</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K149" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="M149" s="24"/>
+      <c r="M149" s="26"/>
       <c r="N149" s="9" t="s">
         <v>102</v>
       </c>
@@ -11397,14 +11807,14 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="U149" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="V149" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="V149" s="2" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="150" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B150" s="24"/>
+      <c r="B150" s="26"/>
       <c r="C150" s="9" t="s">
         <v>103</v>
       </c>
@@ -11432,9 +11842,13 @@
         <f t="shared" si="92"/>
         <v>0.63800000000000001</v>
       </c>
-      <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
-      <c r="M150" s="24"/>
+      <c r="J150" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K150" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="M150" s="26"/>
       <c r="N150" s="9" t="s">
         <v>103</v>
       </c>
@@ -11462,61 +11876,15 @@
         <f t="shared" ref="T150" si="98">(T145+T146+T147+T148+T149)/5</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="U150" s="2"/>
-      <c r="V150" s="2"/>
+      <c r="U150" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="V150" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="M20:M25"/>
-    <mergeCell ref="M26:M31"/>
-    <mergeCell ref="M62:M67"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="M44:M49"/>
-    <mergeCell ref="M50:M55"/>
-    <mergeCell ref="M56:M61"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="B50:B55"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="M32:M37"/>
-    <mergeCell ref="M38:M43"/>
-    <mergeCell ref="M14:M19"/>
-    <mergeCell ref="O82:Q82"/>
-    <mergeCell ref="R82:T82"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="B97:B102"/>
-    <mergeCell ref="M97:M102"/>
-    <mergeCell ref="M68:M73"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="U84:V84"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="M85:M90"/>
-    <mergeCell ref="B91:B96"/>
-    <mergeCell ref="M91:M96"/>
-    <mergeCell ref="B103:B108"/>
-    <mergeCell ref="M103:M108"/>
-    <mergeCell ref="B109:B114"/>
-    <mergeCell ref="M109:M114"/>
-    <mergeCell ref="B115:B120"/>
-    <mergeCell ref="M115:M120"/>
     <mergeCell ref="B139:B144"/>
     <mergeCell ref="M139:M144"/>
     <mergeCell ref="B145:B150"/>
@@ -11527,6 +11895,56 @@
     <mergeCell ref="M127:M132"/>
     <mergeCell ref="B133:B138"/>
     <mergeCell ref="M133:M138"/>
+    <mergeCell ref="B103:B108"/>
+    <mergeCell ref="M103:M108"/>
+    <mergeCell ref="B109:B114"/>
+    <mergeCell ref="M109:M114"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="M115:M120"/>
+    <mergeCell ref="U84:V84"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="M85:M90"/>
+    <mergeCell ref="B91:B96"/>
+    <mergeCell ref="M91:M96"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="M97:M102"/>
+    <mergeCell ref="M68:M73"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="O82:Q82"/>
+    <mergeCell ref="R82:T82"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="M32:M37"/>
+    <mergeCell ref="M14:M19"/>
+    <mergeCell ref="M20:M25"/>
+    <mergeCell ref="M26:M31"/>
+    <mergeCell ref="M62:M67"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="M44:M49"/>
+    <mergeCell ref="M50:M55"/>
+    <mergeCell ref="M56:M61"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="M38:M43"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="M7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>